<commit_message>
Further text on Data Preparation in Report
</commit_message>
<xml_diff>
--- a/Excel/WineDataset_Training_and_Test_Split_Check cf v1-0 300120.xlsx
+++ b/Excel/WineDataset_Training_and_Test_Split_Check cf v1-0 300120.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Training</t>
   </si>
@@ -64,13 +64,22 @@
   </si>
   <si>
     <t>Wine Quality</t>
+  </si>
+  <si>
+    <t>+300 minority rows</t>
+  </si>
+  <si>
+    <t>+200 minority rows</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +105,14 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -145,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -153,6 +170,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,17 +481,18 @@
   <dimension ref="A2:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="A2" sqref="A2:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" customWidth="1"/>
-    <col min="5" max="5" width="3.21875" customWidth="1"/>
-    <col min="6" max="8" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.77734375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="3.21875" hidden="1" customWidth="1"/>
+    <col min="6" max="8" width="25.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="2.88671875" hidden="1" customWidth="1"/>
     <col min="10" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.6640625" customWidth="1"/>
   </cols>
@@ -477,21 +501,21 @@
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="2"/>
@@ -515,6 +539,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
@@ -616,7 +651,29 @@
         <v>100</v>
       </c>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J11" s="6">
+        <f>(J4+J8)/$B$12</f>
+        <v>0.53619302949061665</v>
+      </c>
+      <c r="K11" s="6">
+        <f>(K4+K8)/$B$12</f>
+        <v>0.35746201966041108</v>
+      </c>
+      <c r="L11" s="6">
+        <f>(L4+L8)/$B$12</f>
+        <v>0.17873100983020554</v>
+      </c>
+    </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
       <c r="B12" s="3">
         <f>SUM(B4:B11)</f>
         <v>1119</v>
@@ -639,25 +696,6 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J14" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J15" s="6">
-        <f>(J4+J8)/$B$12</f>
-        <v>0.53619302949061665</v>
-      </c>
-      <c r="K15" s="6">
-        <f t="shared" ref="K15:L15" si="1">(K4+K8)/$B$12</f>
-        <v>0.35746201966041108</v>
-      </c>
-      <c r="L15" s="6">
-        <f t="shared" si="1"/>
-        <v>0.17873100983020554</v>
-      </c>
-    </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>

</xml_diff>